<commit_message>
Updating small stuff. Going to try something a bit risky, want it saved somewhere.
</commit_message>
<xml_diff>
--- a/wdiw_hr_after_fill.xlsx
+++ b/wdiw_hr_after_fill.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>Income Group</t>
+  </si>
+  <si>
+    <t>GDP_per_cap</t>
+  </si>
   <si>
     <t>GDP (current US$)</t>
   </si>
@@ -101,6 +110,48 @@
   </si>
   <si>
     <t>Adolescent fertility rate (births per 1,000 women ages 15-19)</t>
+  </si>
+  <si>
+    <t>BLZ</t>
+  </si>
+  <si>
+    <t>BMU</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>CRI</t>
+  </si>
+  <si>
+    <t>SLV</t>
+  </si>
+  <si>
+    <t>GTM</t>
+  </si>
+  <si>
+    <t>HND</t>
+  </si>
+  <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Upper middle income</t>
+  </si>
+  <si>
+    <t>High income</t>
+  </si>
+  <si>
+    <t>Lower middle income</t>
   </si>
 </sst>
 </file>
@@ -458,13 +509,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,929 +603,1040 @@
       <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2">
+    <row r="2" spans="1:32">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>4956.808038981396</v>
+      </c>
+      <c r="D2">
         <v>1862614800</v>
       </c>
-      <c r="B2">
+      <c r="E2">
         <v>1.437288946</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>10.82934861</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>17.7329998</v>
       </c>
-      <c r="E2">
-        <v>13.42014731118855</v>
-      </c>
-      <c r="F2">
+      <c r="H2">
+        <v>13.42014731</v>
+      </c>
+      <c r="I2">
         <v>14.65699959</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>62.90620852</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>67.60900116000001</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>25.97005649262531</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>73.71357728</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>16.47387110916265</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>1.9805288509134</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>375769</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>54.399</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>45.601</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>2.212753796919728</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>13.3</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>28.1</v>
       </c>
-      <c r="U2">
+      <c r="X2">
         <v>41.3</v>
       </c>
-      <c r="V2">
+      <c r="Y2">
         <v>0.3040836880543793</v>
       </c>
-      <c r="W2">
+      <c r="Z2">
         <v>7.5</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <v>22970</v>
       </c>
-      <c r="Y2">
+      <c r="AB2">
         <v>63.72026431</v>
       </c>
-      <c r="Z2">
+      <c r="AC2">
         <v>2.346</v>
       </c>
-      <c r="AA2">
+      <c r="AD2">
         <v>1.150522912663806</v>
       </c>
-      <c r="AB2">
+      <c r="AE2">
         <v>55.08547326</v>
       </c>
-      <c r="AC2">
+      <c r="AF2">
         <v>68.48699999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
-      <c r="A3">
+    <row r="3" spans="1:32">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3">
         <v>6269384</v>
       </c>
-      <c r="B3">
+      <c r="E3">
         <v>4.9</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>0.8</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="H3">
+        <v>4.9</v>
+      </c>
+      <c r="I3">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>66.2</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>86</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>26.1</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>1182.851830961937</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>-1.05491441406553</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
         <v>63874</v>
       </c>
-      <c r="P3">
+      <c r="S3">
         <v>100</v>
       </c>
-      <c r="Q3">
+      <c r="T3">
         <v>-1.060518080266264</v>
       </c>
-      <c r="S3">
+      <c r="V3">
         <v>6.7</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>14.8</v>
       </c>
-      <c r="U3">
+      <c r="X3">
         <v>11</v>
       </c>
-      <c r="V3">
+      <c r="Y3">
         <v>0.2216911419352982</v>
       </c>
-      <c r="X3">
+      <c r="AA3">
         <v>4290</v>
       </c>
-      <c r="Y3">
+      <c r="AB3">
         <v>103.0896604</v>
       </c>
-      <c r="Z3">
+      <c r="AC3">
         <v>1.61</v>
       </c>
-      <c r="AB3">
+      <c r="AE3">
         <v>43</v>
       </c>
-      <c r="AC3">
+      <c r="AF3">
         <v>0.0579</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
-      <c r="A4">
+    <row r="4" spans="1:32">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>45069.92725443246</v>
+      </c>
+      <c r="D4">
         <v>1646870000000</v>
       </c>
-      <c r="B4">
+      <c r="E4">
         <v>25.812</v>
       </c>
-      <c r="C4">
+      <c r="F4">
         <v>1.76095581</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>1.518000007</v>
       </c>
-      <c r="F4">
+      <c r="H4">
+        <v>25.812</v>
+      </c>
+      <c r="I4">
         <v>9.527999879999999</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>69.43000000000001</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>78.95500183</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>12.521239487857</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>52.40331395</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>4.018279850134876</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>1.18592567535081</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>20.21782773233009</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>36540268</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>18.65000000000001</v>
       </c>
-      <c r="P4">
+      <c r="S4">
         <v>81.34999999999999</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <v>1.247407090887428</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>0.5</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>0.2</v>
       </c>
-      <c r="U4">
+      <c r="X4">
         <v>0</v>
       </c>
-      <c r="V4">
+      <c r="Y4">
         <v>0.3125353381008608</v>
       </c>
-      <c r="W4">
+      <c r="Z4">
         <v>2.5</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>9984670</v>
       </c>
-      <c r="Y4">
+      <c r="AB4">
         <v>86.28149306</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>1.4961</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>0.3578112329071835</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>8.61607884</v>
       </c>
-      <c r="AC4">
+      <c r="AF4">
         <v>8.387</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
-      <c r="A5">
+    <row r="5" spans="1:32">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>11752.54360172849</v>
+      </c>
+      <c r="D5">
         <v>58174550212</v>
       </c>
-      <c r="B5">
+      <c r="E5">
         <v>18.99327478</v>
       </c>
-      <c r="C5">
+      <c r="F5">
         <v>5.013778521</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>12.57999992</v>
       </c>
-      <c r="E5">
-        <v>18.99327478118037</v>
-      </c>
-      <c r="F5">
+      <c r="H5">
+        <v>18.99327478</v>
+      </c>
+      <c r="I5">
         <v>18.45000076</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>68.06539651</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>68.97000122</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>13.77717057163327</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>42.76440455</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>96.94386995691343</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>1.02767608960277</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>34.38790603710664</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>4949954</v>
       </c>
-      <c r="O5">
+      <c r="R5">
         <v>21.44</v>
       </c>
-      <c r="P5">
+      <c r="S5">
         <v>78.56</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <v>2.083381079810786</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>48.3</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>1</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>2.7</v>
       </c>
-      <c r="U5">
+      <c r="X5">
         <v>20</v>
       </c>
-      <c r="V5">
+      <c r="Y5">
         <v>0.006479229644173745</v>
       </c>
-      <c r="W5">
+      <c r="Z5">
         <v>4.8</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>51100</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>178.5944273</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>1.772</v>
       </c>
-      <c r="AA5">
+      <c r="AD5">
         <v>0.4292446067561385</v>
       </c>
-      <c r="AB5">
+      <c r="AE5">
         <v>44.56692021</v>
       </c>
-      <c r="AC5">
+      <c r="AF5">
         <v>53.46</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
-      <c r="A6">
+    <row r="6" spans="1:32">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>3902.237621635905</v>
+      </c>
+      <c r="D6">
         <v>24927970000</v>
       </c>
-      <c r="B6">
+      <c r="E6">
         <v>24.44198224</v>
       </c>
-      <c r="C6">
+      <c r="F6">
         <v>5.042047146</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>18.57500076</v>
       </c>
-      <c r="E6">
-        <v>24.44198223922766</v>
-      </c>
-      <c r="F6">
+      <c r="H6">
+        <v>24.44198224</v>
+      </c>
+      <c r="I6">
         <v>21.88599968</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>60.665349</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>59.54000092</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>17.79023005294855</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>65.51676691</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>308.3070463320464</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>0.501858163165851</v>
       </c>
-      <c r="M6">
+      <c r="P6">
         <v>24.25026366454403</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>6388122</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>28.72499999999999</v>
       </c>
-      <c r="P6">
+      <c r="S6">
         <v>71.27500000000001</v>
       </c>
-      <c r="Q6">
+      <c r="T6">
         <v>1.593741609219283</v>
       </c>
-      <c r="R6">
+      <c r="U6">
         <v>38</v>
       </c>
-      <c r="S6">
+      <c r="V6">
         <v>1.9</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>8.5</v>
       </c>
-      <c r="U6">
+      <c r="X6">
         <v>29.2</v>
       </c>
-      <c r="V6">
+      <c r="Y6">
         <v>0.4354211462967214</v>
       </c>
-      <c r="W6">
+      <c r="Z6">
         <v>9</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>21040</v>
       </c>
-      <c r="Y6">
+      <c r="AB6">
         <v>148.3697097</v>
       </c>
-      <c r="Z6">
+      <c r="AC6">
         <v>2.059</v>
       </c>
-      <c r="AA6">
+      <c r="AD6">
         <v>1.489587781407958</v>
       </c>
-      <c r="AB6">
+      <c r="AE6">
         <v>55.15985313</v>
       </c>
-      <c r="AC6">
+      <c r="AF6">
         <v>69.459</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
-      <c r="A7">
+    <row r="7" spans="1:32">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>4470.610798497878</v>
+      </c>
+      <c r="D7">
         <v>75620095538</v>
       </c>
-      <c r="B7">
+      <c r="E7">
         <v>5.26910429</v>
       </c>
-      <c r="C7">
+      <c r="F7">
         <v>10.05815003</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>29.31599998</v>
       </c>
-      <c r="E7">
-        <v>25.26910428509802</v>
-      </c>
-      <c r="F7">
+      <c r="H7">
+        <v>25.26910429</v>
+      </c>
+      <c r="I7">
         <v>20.89800072</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>62.13797562</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>49.7859993</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>38.86533043</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>157.8474804031355</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>1.9815326212916</v>
       </c>
-      <c r="M7">
+      <c r="P7">
         <v>32.814456476473</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <v>16914936</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <v>49.32</v>
       </c>
-      <c r="P7">
+      <c r="S7">
         <v>50.68</v>
       </c>
-      <c r="Q7">
+      <c r="T7">
         <v>2.696398842633449</v>
       </c>
-      <c r="S7">
+      <c r="V7">
         <v>8.699999999999999</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>24.2</v>
       </c>
-      <c r="U7">
+      <c r="X7">
         <v>59.3</v>
       </c>
-      <c r="V7">
+      <c r="Y7">
         <v>0.4703566567812231</v>
       </c>
-      <c r="W7">
+      <c r="Z7">
         <v>15.2</v>
       </c>
-      <c r="X7">
+      <c r="AA7">
         <v>108890</v>
       </c>
-      <c r="Y7">
+      <c r="AB7">
         <v>118.1585424</v>
       </c>
-      <c r="Z7">
+      <c r="AC7">
         <v>2.92</v>
       </c>
-      <c r="AA7">
+      <c r="AD7">
         <v>0.6285589409220375</v>
       </c>
-      <c r="AB7">
+      <c r="AE7">
         <v>65.96741609999999</v>
       </c>
-      <c r="AC7">
+      <c r="AF7">
         <v>70.93000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8">
+    <row r="8" spans="1:32">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>2432.935363819599</v>
+      </c>
+      <c r="D8">
         <v>22940179174</v>
       </c>
-      <c r="B8">
+      <c r="E8">
         <v>6.47477854</v>
       </c>
-      <c r="C8">
+      <c r="F8">
         <v>12.84493271</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>31.98500061</v>
       </c>
-      <c r="E8">
-        <v>26.47477853532524</v>
-      </c>
-      <c r="F8">
+      <c r="H8">
+        <v>26.47477854</v>
+      </c>
+      <c r="I8">
         <v>20.68300056</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>56.82448851</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>47.33200073</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>87.17891804</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>84.27038162481008</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>1.6922288789459</v>
       </c>
-      <c r="M8">
+      <c r="P8">
         <v>24.76290252469409</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <v>9429013</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>43.543</v>
       </c>
-      <c r="P8">
+      <c r="S8">
         <v>56.457</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <v>2.839474653621561</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>50.5</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>17.2</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>31.6</v>
       </c>
-      <c r="U8">
+      <c r="X8">
         <v>64.3</v>
       </c>
-      <c r="V8">
+      <c r="Y8">
         <v>0.4687533313088352</v>
       </c>
-      <c r="W8">
+      <c r="Z8">
         <v>12.9</v>
       </c>
-      <c r="X8">
+      <c r="AA8">
         <v>112490</v>
       </c>
-      <c r="Y8">
+      <c r="AB8">
         <v>87.32089987000001</v>
       </c>
-      <c r="Z8">
+      <c r="AC8">
         <v>2.496</v>
       </c>
-      <c r="AA8">
+      <c r="AD8">
         <v>0.552978329260127</v>
       </c>
-      <c r="AB8">
+      <c r="AE8">
         <v>58.49347529</v>
       </c>
-      <c r="AC8">
+      <c r="AF8">
         <v>72.91200000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
-      <c r="A9">
+    <row r="9" spans="1:32">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>9281.101482907432</v>
+      </c>
+      <c r="D9">
         <v>1158070000000</v>
       </c>
-      <c r="B9">
+      <c r="E9">
         <v>30.70067888</v>
       </c>
-      <c r="C9">
+      <c r="F9">
         <v>3.380989702</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>13.11800003</v>
       </c>
-      <c r="E9">
-        <v>30.70067888140514</v>
-      </c>
-      <c r="F9">
+      <c r="H9">
+        <v>30.70067888</v>
+      </c>
+      <c r="I9">
         <v>26.01300049</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>60.36615614</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>60.86999893</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>13.04335905791983</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>72.66860106999999</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>64.18751716865145</v>
       </c>
-      <c r="L9">
+      <c r="O9">
         <v>1.16396777921201</v>
       </c>
-      <c r="M9">
+      <c r="P9">
         <v>21.57448773356682</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <v>124777324</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>20.133</v>
       </c>
-      <c r="P9">
+      <c r="S9">
         <v>79.867</v>
       </c>
-      <c r="Q9">
+      <c r="T9">
         <v>1.527731512523876</v>
       </c>
-      <c r="S9">
+      <c r="V9">
         <v>3.2</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>7.9</v>
       </c>
-      <c r="U9">
+      <c r="X9">
         <v>50.6</v>
       </c>
-      <c r="V9">
+      <c r="Y9">
         <v>0.1751380871908623</v>
       </c>
-      <c r="W9">
+      <c r="Z9">
         <v>3.6</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>1964375</v>
       </c>
-      <c r="Y9">
+      <c r="AB9">
         <v>91.62670695</v>
       </c>
-      <c r="Z9">
+      <c r="AC9">
         <v>2.157</v>
       </c>
-      <c r="AA9">
+      <c r="AD9">
         <v>0.6032825465188298</v>
       </c>
-      <c r="AB9">
+      <c r="AE9">
         <v>51.46924127</v>
       </c>
-      <c r="AC9">
+      <c r="AF9">
         <v>60.365</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
-      <c r="A10">
+    <row r="10" spans="1:32">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>2168.191239979627</v>
+      </c>
+      <c r="D10">
         <v>13843586680</v>
       </c>
-      <c r="B10">
+      <c r="E10">
         <v>24.99016119</v>
       </c>
-      <c r="C10">
+      <c r="F10">
         <v>15.07211843</v>
       </c>
-      <c r="D10">
+      <c r="G10">
         <v>31.0909996</v>
       </c>
-      <c r="E10">
-        <v>24.99016118751795</v>
-      </c>
-      <c r="F10">
+      <c r="H10">
+        <v>24.99016119</v>
+      </c>
+      <c r="I10">
         <v>16.93899918</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>50.13167656</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>51.97000122</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>16.50469592747782</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>90.11392993</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>53.05679740734585</v>
       </c>
-      <c r="L10">
+      <c r="O10">
         <v>1.27485515697153</v>
       </c>
-      <c r="M10">
+      <c r="P10">
         <v>27.95975721508194</v>
       </c>
-      <c r="N10">
+      <c r="Q10">
         <v>6384855</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <v>41.701</v>
       </c>
-      <c r="P10">
+      <c r="S10">
         <v>58.299</v>
       </c>
-      <c r="Q10">
+      <c r="T10">
         <v>1.634019876665461</v>
       </c>
-      <c r="S10">
+      <c r="V10">
         <v>2.5</v>
       </c>
-      <c r="T10">
+      <c r="W10">
         <v>12.8</v>
       </c>
-      <c r="U10">
+      <c r="X10">
         <v>24.9</v>
       </c>
-      <c r="V10">
+      <c r="Y10">
         <v>0.2887971853240742</v>
       </c>
-      <c r="W10">
+      <c r="Z10">
         <v>17</v>
       </c>
-      <c r="X10">
+      <c r="AA10">
         <v>130370</v>
       </c>
-      <c r="Y10">
+      <c r="AB10">
         <v>128.1139122</v>
       </c>
-      <c r="Z10">
+      <c r="AC10">
         <v>2.43</v>
       </c>
-      <c r="AA10">
+      <c r="AD10">
         <v>0.4066488441514916</v>
       </c>
-      <c r="AB10">
+      <c r="AE10">
         <v>5.28115039</v>
       </c>
-      <c r="AC10">
+      <c r="AF10">
         <v>84.98999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
-      <c r="A11">
+    <row r="11" spans="1:32">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>15166.12443206597</v>
+      </c>
+      <c r="D11">
         <v>62283800000</v>
       </c>
-      <c r="B11">
+      <c r="E11">
         <v>29.34470922</v>
       </c>
-      <c r="C11">
+      <c r="F11">
         <v>2.357434839</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>14.49400043</v>
       </c>
-      <c r="E11">
-        <v>29.34470921812734</v>
-      </c>
-      <c r="F11">
+      <c r="H11">
+        <v>29.34470922</v>
+      </c>
+      <c r="I11">
         <v>18.54899979</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>64.64971629999999</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>66.95600128</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>53.03465749</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>55.24308582189938</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>1.71159119963697</v>
       </c>
-      <c r="M11">
+      <c r="P11">
         <v>63.10849780555108</v>
       </c>
-      <c r="N11">
+      <c r="Q11">
         <v>4106771</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <v>32.63500000000001</v>
       </c>
-      <c r="P11">
+      <c r="S11">
         <v>67.36499999999999</v>
       </c>
-      <c r="Q11">
+      <c r="T11">
         <v>2.214598137773381</v>
       </c>
-      <c r="R11">
+      <c r="U11">
         <v>49.9</v>
       </c>
-      <c r="S11">
+      <c r="V11">
         <v>2.5</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>6.3</v>
       </c>
-      <c r="U11">
+      <c r="X11">
         <v>22.1</v>
       </c>
-      <c r="V11">
+      <c r="Y11">
         <v>0.3003437889972702</v>
       </c>
-      <c r="W11">
+      <c r="Z11">
         <v>10</v>
       </c>
-      <c r="X11">
+      <c r="AA11">
         <v>75420</v>
       </c>
-      <c r="Y11">
+      <c r="AB11">
         <v>128.5729731</v>
       </c>
-      <c r="Z11">
+      <c r="AC11">
         <v>2.487</v>
       </c>
-      <c r="AA11">
+      <c r="AD11">
         <v>1.311152664564788</v>
       </c>
-      <c r="AB11">
+      <c r="AE11">
         <v>54.4387154</v>
       </c>
-      <c r="AC11">
+      <c r="AF11">
         <v>81.828</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
-      <c r="A12">
+    <row r="12" spans="1:32">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <v>59927.92983395354</v>
+      </c>
+      <c r="D12">
         <v>19485400000000</v>
       </c>
-      <c r="B12">
+      <c r="E12">
         <v>18.20794002</v>
       </c>
-      <c r="C12">
+      <c r="F12">
         <v>0.91647932</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>1.434999943</v>
       </c>
-      <c r="E12">
-        <v>18.20794001787016</v>
-      </c>
-      <c r="F12">
+      <c r="H12">
+        <v>18.20794002</v>
+      </c>
+      <c r="I12">
         <v>19.72900009</v>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>77.37453175</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>78.83599854000001</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>11.94741054536897</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>0.29596645</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>35.54522706949063</v>
       </c>
-      <c r="L12">
+      <c r="O12">
         <v>0.640458800224899</v>
       </c>
-      <c r="M12">
+      <c r="P12">
         <v>7.031968628520996</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <v>325147121</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <v>17.94199999999999</v>
       </c>
-      <c r="P12">
+      <c r="S12">
         <v>82.05800000000001</v>
       </c>
-      <c r="Q12">
+      <c r="T12">
         <v>0.8796001226745864</v>
       </c>
-      <c r="S12">
+      <c r="V12">
         <v>1.2</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>1.5</v>
       </c>
-      <c r="U12">
+      <c r="X12">
         <v>0</v>
       </c>
-      <c r="V12">
+      <c r="Y12">
         <v>0.2756080342194764</v>
       </c>
-      <c r="W12">
+      <c r="Z12">
         <v>2.5</v>
       </c>
-      <c r="X12">
+      <c r="AA12">
         <v>9831510</v>
       </c>
-      <c r="Y12">
+      <c r="AB12">
         <v>123.10815</v>
       </c>
-      <c r="Z12">
+      <c r="AC12">
         <v>1.7655</v>
       </c>
-      <c r="AA12">
+      <c r="AD12">
         <v>0.8269084302718168</v>
       </c>
-      <c r="AB12">
+      <c r="AE12">
         <v>52.1558055</v>
       </c>
-      <c r="AC12">
+      <c r="AF12">
         <v>19.86</v>
       </c>
     </row>

</xml_diff>